<commit_message>
fixed votes primary key
</commit_message>
<xml_diff>
--- a/election/src/main/resources/database/election-inserts.xlsx
+++ b/election/src/main/resources/database/election-inserts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GraduateStudies\db_systems\final-project-repo\election\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GraduateStudies\db_systems\final-project-repo\election\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F148003-7742-4A83-AA44-570E77B012C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E974543-6462-4CEF-B3B9-0BF94C983648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{CF11789D-A1C1-4EA3-82EE-040757E1459A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{CF11789D-A1C1-4EA3-82EE-040757E1459A}"/>
   </bookViews>
   <sheets>
     <sheet name="ELECTION" sheetId="1" r:id="rId1"/>
@@ -783,10 +783,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1674,16 +1673,16 @@
       <c r="A10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1710,16 +1709,16 @@
       <c r="A11" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>213</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -1746,16 +1745,16 @@
       <c r="A12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>214</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1782,16 +1781,16 @@
       <c r="A13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>215</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1818,16 +1817,16 @@
       <c r="A14" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>216</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1854,16 +1853,16 @@
       <c r="A15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>217</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1890,16 +1889,16 @@
       <c r="A16" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>218</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1926,16 +1925,16 @@
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>221</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1962,16 +1961,16 @@
       <c r="A18" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>219</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1998,16 +1997,16 @@
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>220</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -2043,7 +2042,7 @@
       <c r="D20" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>222</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -2079,7 +2078,7 @@
       <c r="D21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>223</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2115,7 +2114,7 @@
       <c r="D22" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>224</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -2151,7 +2150,7 @@
       <c r="D23" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>225</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -2187,7 +2186,7 @@
       <c r="D24" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>226</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -2223,7 +2222,7 @@
       <c r="D25" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>227</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -2259,7 +2258,7 @@
       <c r="D26" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>228</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -2295,7 +2294,7 @@
       <c r="D27" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>229</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -2366,7 +2365,7 @@
         <v>94</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C12" si="0">CONCATENATE( "INSERT INTO OFFICE VALUES(", A3, ",", B3, ");")</f>
+        <f t="shared" ref="C3:C10" si="0">CONCATENATE( "INSERT INTO OFFICE VALUES(", A3, ",", B3, ");")</f>
         <v>INSERT INTO OFFICE VALUES(91,'City Attorney');</v>
       </c>
     </row>
@@ -3520,8 +3519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F1C548-88B6-4D52-821D-479EDF6DFA13}">
   <dimension ref="A1:D235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="O208" sqref="O208"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,8 +3553,8 @@
         <v>5</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE("INSERT INTO VOTES VALUES(",A2, ",", B2, ",", C2, ");")</f>
-        <v>INSERT INTO VOTES VALUES(1,12,3);</v>
+        <f>CONCATENATE("INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(",A2, ",", B2, ",", C2, ");")</f>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,12,3);</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3569,8 +3568,8 @@
         <v>5</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">CONCATENATE("INSERT INTO VOTES VALUES(",A3, ",", B3, ",", C3, ");")</f>
-        <v>INSERT INTO VOTES VALUES(2,11,3);</v>
+        <f t="shared" ref="D3:D66" si="0">CONCATENATE("INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(",A3, ",", B3, ",", C3, ");")</f>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,11,3);</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3585,7 +3584,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,12,3);</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,7 +3599,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,13,3);</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3614,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,14,3);</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,7 +3629,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,11,3);</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3645,7 +3644,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,14,3);</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3660,7 +3659,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,13,3);</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3675,7 +3674,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,14,3);</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3690,7 +3689,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,11,3);</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,7 +3704,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,14,3);</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3720,7 +3719,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,13,3);</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3735,7 +3734,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,12,3);</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,7 +3749,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,11,3);</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3765,7 +3764,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,13,3);</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3780,7 +3779,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,11,3);</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3795,7 +3794,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,12,3);</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,7 +3809,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,13,3);</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3825,7 +3824,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,13,3);</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3840,7 +3839,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,13,3);</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3855,7 +3854,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,11,3);</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,7 +3869,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,12,3);</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3885,7 +3884,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,14,3);</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3900,7 +3899,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,14,3);</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3915,7 +3914,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(2,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(2,13,3);</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3930,7 +3929,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(1,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(1,14,3);</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3945,7 +3944,7 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,13,3);</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3960,7 +3959,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,12,3);</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,7 +3974,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,14,3);</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3990,7 +3989,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,14,3);</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4005,7 +4004,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,13,3);</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4020,7 +4019,7 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,12,3);</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4035,7 +4034,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,14,3);</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4050,7 +4049,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,12,3);</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4065,7 +4064,7 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,14,3);</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4080,7 +4079,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,14,3);</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4095,7 +4094,7 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,11,3);</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,7 +4109,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,11,3);</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4125,7 +4124,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,11,3);</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4140,7 +4139,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,11,3);</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4155,7 +4154,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,12,3);</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4170,7 +4169,7 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,11,3);</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4185,7 +4184,7 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,11,3);</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4200,7 +4199,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,13,3);</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4215,7 +4214,7 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,13,3);</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4230,7 +4229,7 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,14,3);</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4245,7 +4244,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,14,3);</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4260,7 +4259,7 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,12,3);</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,7 +4274,7 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,14,3);</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4290,7 +4289,7 @@
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,13,3);</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4305,7 +4304,7 @@
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(4,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(4,12,3);</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4320,7 +4319,7 @@
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(3,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(3,14,3);</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4335,7 +4334,7 @@
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(5,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,13,3);</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4350,7 +4349,7 @@
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,14,3);</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4365,7 +4364,7 @@
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,14,3);</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4380,7 +4379,7 @@
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(5,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,11,3);</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4395,7 +4394,7 @@
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4410,7 +4409,7 @@
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,14,3);</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +4424,7 @@
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4440,7 +4439,7 @@
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(5,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,12,3);</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4455,7 +4454,7 @@
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,13,3);</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4470,7 +4469,7 @@
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(5,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,11,3);</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4485,7 +4484,7 @@
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4500,7 +4499,7 @@
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,7 +4514,7 @@
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO VOTES VALUES(6,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,13,3);</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4529,8 +4528,8 @@
         <v>5</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D130" si="1">CONCATENATE("INSERT INTO VOTES VALUES(",A67, ",", B67, ",", C67, ");")</f>
-        <v>INSERT INTO VOTES VALUES(5,12,3);</v>
+        <f t="shared" ref="D67:D130" si="1">CONCATENATE("INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(",A67, ",", B67, ",", C67, ");")</f>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,12,3);</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4545,7 +4544,7 @@
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,11,3);</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4560,7 +4559,7 @@
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -4575,7 +4574,7 @@
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4590,7 +4589,7 @@
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,14,3);</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4605,7 +4604,7 @@
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(6,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,12,3);</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4620,7 +4619,7 @@
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4635,7 +4634,7 @@
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,13,3);</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4650,7 +4649,7 @@
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,14,3);</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4665,7 +4664,7 @@
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,12,3);</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4680,7 +4679,7 @@
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,13,3);</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4695,7 +4694,7 @@
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(5,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(5,12,3);</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4710,7 +4709,7 @@
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(6,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(6,11,3);</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4725,7 +4724,7 @@
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,13,3);</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4740,7 +4739,7 @@
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,14,3);</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,7 +4754,7 @@
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,14,3);</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4770,7 +4769,7 @@
       </c>
       <c r="D83" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,13,3);</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,7 +4784,7 @@
       </c>
       <c r="D84" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,14,3);</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4800,7 +4799,7 @@
       </c>
       <c r="D85" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,12,3);</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4815,7 +4814,7 @@
       </c>
       <c r="D86" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,12,3);</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4830,7 +4829,7 @@
       </c>
       <c r="D87" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,11,3);</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4845,7 +4844,7 @@
       </c>
       <c r="D88" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,13,3);</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,7 +4859,7 @@
       </c>
       <c r="D89" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,11,3);</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4875,7 +4874,7 @@
       </c>
       <c r="D90" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,11,3);</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4890,7 +4889,7 @@
       </c>
       <c r="D91" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,11,3);</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4905,7 +4904,7 @@
       </c>
       <c r="D92" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,13,3);</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4920,7 +4919,7 @@
       </c>
       <c r="D93" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,11,3);</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4935,7 +4934,7 @@
       </c>
       <c r="D94" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,14,3);</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4950,7 +4949,7 @@
       </c>
       <c r="D95" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,11,3);</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4965,7 +4964,7 @@
       </c>
       <c r="D96" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,14,3);</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4980,7 +4979,7 @@
       </c>
       <c r="D97" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,11,3);</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,7 +4994,7 @@
       </c>
       <c r="D98" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,12,3);</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -5010,7 +5009,7 @@
       </c>
       <c r="D99" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,14,3);</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -5025,7 +5024,7 @@
       </c>
       <c r="D100" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,12,3);</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -5040,7 +5039,7 @@
       </c>
       <c r="D101" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,12,3);</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -5055,7 +5054,7 @@
       </c>
       <c r="D102" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,13,3);</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -5070,7 +5069,7 @@
       </c>
       <c r="D103" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,11,3);</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -5085,7 +5084,7 @@
       </c>
       <c r="D104" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(7,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(7,12,3);</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -5100,7 +5099,7 @@
       </c>
       <c r="D105" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(8,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(8,12,3);</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -5115,7 +5114,7 @@
       </c>
       <c r="D106" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,11,3);</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -5130,7 +5129,7 @@
       </c>
       <c r="D107" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,11,3);</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -5145,7 +5144,7 @@
       </c>
       <c r="D108" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,12,3);</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -5160,7 +5159,7 @@
       </c>
       <c r="D109" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,12,3);</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -5175,7 +5174,7 @@
       </c>
       <c r="D110" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,14,3);</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -5190,7 +5189,7 @@
       </c>
       <c r="D111" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,11,3);</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5205,7 +5204,7 @@
       </c>
       <c r="D112" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,11,3);</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -5220,7 +5219,7 @@
       </c>
       <c r="D113" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,12,3);</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5235,7 +5234,7 @@
       </c>
       <c r="D114" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,11,3);</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -5250,7 +5249,7 @@
       </c>
       <c r="D115" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,14,3);</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -5265,7 +5264,7 @@
       </c>
       <c r="D116" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,14,3);</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5280,7 +5279,7 @@
       </c>
       <c r="D117" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,11,3);</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5295,7 +5294,7 @@
       </c>
       <c r="D118" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,11,3);</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5310,7 +5309,7 @@
       </c>
       <c r="D119" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,14,3);</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5325,7 +5324,7 @@
       </c>
       <c r="D120" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,12,3);</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5340,7 +5339,7 @@
       </c>
       <c r="D121" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,11,3);</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5355,7 +5354,7 @@
       </c>
       <c r="D122" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,13,3);</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -5370,7 +5369,7 @@
       </c>
       <c r="D123" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,12,3);</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5385,7 +5384,7 @@
       </c>
       <c r="D124" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,13,3);</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5400,7 +5399,7 @@
       </c>
       <c r="D125" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,12,3);</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5415,7 +5414,7 @@
       </c>
       <c r="D126" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,11,3);</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -5430,7 +5429,7 @@
       </c>
       <c r="D127" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,14,3);</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5445,7 +5444,7 @@
       </c>
       <c r="D128" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,13,3);</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5460,7 +5459,7 @@
       </c>
       <c r="D129" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(10,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(10,11,3);</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5475,7 +5474,7 @@
       </c>
       <c r="D130" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO VOTES VALUES(9,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,12,3);</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5489,8 +5488,8 @@
         <v>5</v>
       </c>
       <c r="D131" t="str">
-        <f t="shared" ref="D131:D194" si="2">CONCATENATE("INSERT INTO VOTES VALUES(",A131, ",", B131, ",", C131, ");")</f>
-        <v>INSERT INTO VOTES VALUES(9,11,3);</v>
+        <f t="shared" ref="D131:D194" si="2">CONCATENATE("INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(",A131, ",", B131, ",", C131, ");")</f>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(9,11,3);</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5505,7 +5504,7 @@
       </c>
       <c r="D132" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,13,3);</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5520,7 +5519,7 @@
       </c>
       <c r="D133" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,11,3);</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5535,7 +5534,7 @@
       </c>
       <c r="D134" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,13,3);</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5550,7 +5549,7 @@
       </c>
       <c r="D135" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,13,3);</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5565,7 +5564,7 @@
       </c>
       <c r="D136" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,13,3);</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5580,7 +5579,7 @@
       </c>
       <c r="D137" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,12,3);</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5595,7 +5594,7 @@
       </c>
       <c r="D138" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -5610,7 +5609,7 @@
       </c>
       <c r="D139" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,14,3);</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -5625,7 +5624,7 @@
       </c>
       <c r="D140" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -5640,7 +5639,7 @@
       </c>
       <c r="D141" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,11,3);</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5655,7 +5654,7 @@
       </c>
       <c r="D142" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,14,3);</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -5670,7 +5669,7 @@
       </c>
       <c r="D143" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5685,7 +5684,7 @@
       </c>
       <c r="D144" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,14,3);</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -5700,7 +5699,7 @@
       </c>
       <c r="D145" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,11,3);</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -5715,7 +5714,7 @@
       </c>
       <c r="D146" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,12,3);</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5730,7 +5729,7 @@
       </c>
       <c r="D147" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5745,7 +5744,7 @@
       </c>
       <c r="D148" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,12,3);</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5760,7 +5759,7 @@
       </c>
       <c r="D149" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,12,3);</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5775,7 +5774,7 @@
       </c>
       <c r="D150" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,14,3);</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5790,7 +5789,7 @@
       </c>
       <c r="D151" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5805,7 +5804,7 @@
       </c>
       <c r="D152" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,11,3);</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5820,7 +5819,7 @@
       </c>
       <c r="D153" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,12,3);</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5835,7 +5834,7 @@
       </c>
       <c r="D154" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(12,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(12,11,3);</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5850,7 +5849,7 @@
       </c>
       <c r="D155" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,13,3);</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5865,7 +5864,7 @@
       </c>
       <c r="D156" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5880,7 +5879,7 @@
       </c>
       <c r="D157" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(11,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(11,11,3);</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -5895,7 +5894,7 @@
       </c>
       <c r="D158" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,13,3);</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5910,7 +5909,7 @@
       </c>
       <c r="D159" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,12,3);</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -5925,7 +5924,7 @@
       </c>
       <c r="D160" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,13,3);</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -5940,7 +5939,7 @@
       </c>
       <c r="D161" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,11,3);</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -5955,7 +5954,7 @@
       </c>
       <c r="D162" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,14,3);</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -5970,7 +5969,7 @@
       </c>
       <c r="D163" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,11,3);</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -5985,7 +5984,7 @@
       </c>
       <c r="D164" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,12,3);</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -6000,7 +5999,7 @@
       </c>
       <c r="D165" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,12,3);</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -6015,7 +6014,7 @@
       </c>
       <c r="D166" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,14,3);</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -6030,7 +6029,7 @@
       </c>
       <c r="D167" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,14,3);</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -6045,7 +6044,7 @@
       </c>
       <c r="D168" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,13,3);</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -6060,7 +6059,7 @@
       </c>
       <c r="D169" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,13,3);</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -6075,7 +6074,7 @@
       </c>
       <c r="D170" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,11,3);</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -6090,7 +6089,7 @@
       </c>
       <c r="D171" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,13,3);</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -6105,7 +6104,7 @@
       </c>
       <c r="D172" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,13,3);</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -6120,7 +6119,7 @@
       </c>
       <c r="D173" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,13,3);</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -6135,7 +6134,7 @@
       </c>
       <c r="D174" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,12,3);</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -6150,7 +6149,7 @@
       </c>
       <c r="D175" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,13,3);</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -6165,7 +6164,7 @@
       </c>
       <c r="D176" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,14,3);</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -6180,7 +6179,7 @@
       </c>
       <c r="D177" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,12,3);</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -6195,7 +6194,7 @@
       </c>
       <c r="D178" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,14,3);</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -6210,7 +6209,7 @@
       </c>
       <c r="D179" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,13,3);</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -6225,7 +6224,7 @@
       </c>
       <c r="D180" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,12,3);</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -6240,7 +6239,7 @@
       </c>
       <c r="D181" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,14,3);</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -6255,7 +6254,7 @@
       </c>
       <c r="D182" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(13,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(13,11,3);</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -6270,7 +6269,7 @@
       </c>
       <c r="D183" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(14,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(14,11,3);</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -6285,7 +6284,7 @@
       </c>
       <c r="D184" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,11,3);</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -6300,7 +6299,7 @@
       </c>
       <c r="D185" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,13,3);</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -6315,7 +6314,7 @@
       </c>
       <c r="D186" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,13,3);</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -6330,7 +6329,7 @@
       </c>
       <c r="D187" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,14,3);</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -6345,7 +6344,7 @@
       </c>
       <c r="D188" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,11,3);</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -6360,7 +6359,7 @@
       </c>
       <c r="D189" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(15,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,11,3);</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -6375,7 +6374,7 @@
       </c>
       <c r="D190" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(15,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,11,3);</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -6390,7 +6389,7 @@
       </c>
       <c r="D191" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(15,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,11,3);</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -6405,7 +6404,7 @@
       </c>
       <c r="D192" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,14,3);</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -6420,7 +6419,7 @@
       </c>
       <c r="D193" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,12,3);</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -6435,7 +6434,7 @@
       </c>
       <c r="D194" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO VOTES VALUES(16,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,12,3);</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -6449,8 +6448,8 @@
         <v>5</v>
       </c>
       <c r="D195" t="str">
-        <f t="shared" ref="D195:D235" si="3">CONCATENATE("INSERT INTO VOTES VALUES(",A195, ",", B195, ",", C195, ");")</f>
-        <v>INSERT INTO VOTES VALUES(15,11,3);</v>
+        <f t="shared" ref="D195:D235" si="3">CONCATENATE("INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(",A195, ",", B195, ",", C195, ");")</f>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,11,3);</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -6465,7 +6464,7 @@
       </c>
       <c r="D196" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,14,3);</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -6480,7 +6479,7 @@
       </c>
       <c r="D197" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,12,3);</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -6495,7 +6494,7 @@
       </c>
       <c r="D198" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,13,3);</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -6510,7 +6509,7 @@
       </c>
       <c r="D199" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,14,3);</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -6525,7 +6524,7 @@
       </c>
       <c r="D200" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,14,3);</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -6540,7 +6539,7 @@
       </c>
       <c r="D201" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,11,3);</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -6555,7 +6554,7 @@
       </c>
       <c r="D202" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,11,3);</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -6570,7 +6569,7 @@
       </c>
       <c r="D203" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,12,3);</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -6585,7 +6584,7 @@
       </c>
       <c r="D204" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,14,3);</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -6600,7 +6599,7 @@
       </c>
       <c r="D205" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,11,3);</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -6615,7 +6614,7 @@
       </c>
       <c r="D206" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,13,3);</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -6630,7 +6629,7 @@
       </c>
       <c r="D207" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(16,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(16,11,3);</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -6645,7 +6644,7 @@
       </c>
       <c r="D208" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,14,3);</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -6660,7 +6659,7 @@
       </c>
       <c r="D209" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(15,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(15,11,3);</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -6675,7 +6674,7 @@
       </c>
       <c r="D210" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,13,3);</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -6690,7 +6689,7 @@
       </c>
       <c r="D211" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,12,3);</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -6705,7 +6704,7 @@
       </c>
       <c r="D212" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,12,3);</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -6720,7 +6719,7 @@
       </c>
       <c r="D213" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,12,3);</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -6735,7 +6734,7 @@
       </c>
       <c r="D214" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,11,3);</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -6750,7 +6749,7 @@
       </c>
       <c r="D215" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,13,3);</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -6765,7 +6764,7 @@
       </c>
       <c r="D216" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,14,3);</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -6780,7 +6779,7 @@
       </c>
       <c r="D217" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,14,3);</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -6795,7 +6794,7 @@
       </c>
       <c r="D218" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,14,3);</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -6810,7 +6809,7 @@
       </c>
       <c r="D219" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,11,3);</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -6825,7 +6824,7 @@
       </c>
       <c r="D220" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,13,3);</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -6840,7 +6839,7 @@
       </c>
       <c r="D221" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,14,3);</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -6855,7 +6854,7 @@
       </c>
       <c r="D222" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,13,3);</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -6870,7 +6869,7 @@
       </c>
       <c r="D223" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,13,3);</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -6885,7 +6884,7 @@
       </c>
       <c r="D224" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,12,3);</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -6900,7 +6899,7 @@
       </c>
       <c r="D225" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,14,3);</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -6915,7 +6914,7 @@
       </c>
       <c r="D226" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,13,3);</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -6930,7 +6929,7 @@
       </c>
       <c r="D227" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,12,3);</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -6945,7 +6944,7 @@
       </c>
       <c r="D228" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,13,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,13,3);</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -6960,7 +6959,7 @@
       </c>
       <c r="D229" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,14,3);</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -6975,7 +6974,7 @@
       </c>
       <c r="D230" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,14,3);</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -6990,7 +6989,7 @@
       </c>
       <c r="D231" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,14,3);</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -7005,7 +7004,7 @@
       </c>
       <c r="D232" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,11,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,11,3);</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -7020,7 +7019,7 @@
       </c>
       <c r="D233" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(17,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(17,12,3);</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -7035,7 +7034,7 @@
       </c>
       <c r="D234" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,12,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,12,3);</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -7050,7 +7049,7 @@
       </c>
       <c r="D235" t="str">
         <f t="shared" si="3"/>
-        <v>INSERT INTO VOTES VALUES(18,14,3);</v>
+        <v>INSERT INTO VOTES(candidate_id, poll_id, election_id) VALUES(18,14,3);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>